<commit_message>
#2817 /  #2818 - Data Importer fixes and enhancements
</commit_message>
<xml_diff>
--- a/bundle/src/test/resources/com/adobe/acs/commons/mcp/impl/processes/data-importer.xlsx
+++ b/bundle/src/test/resources/com/adobe/acs/commons/mcp/impl/processes/data-importer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brobert\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidg/Code/acs-aem-commons/bundle/src/test/resources/com/adobe/acs/commons/mcp/impl/processes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16A6E1C-5A54-43B8-A28D-55C543D5BE8F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A12804D3-2E20-C14B-9E2F-74908ED9CDD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" xr2:uid="{B989199F-66C5-4B28-BA4B-596AA9AB6E6A}"/>
+    <workbookView xWindow="22620" yWindow="14120" windowWidth="34140" windowHeight="12140" xr2:uid="{B989199F-66C5-4B28-BA4B-596AA9AB6E6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>This is just a regular string</t>
   </si>
@@ -81,6 +86,15 @@
   </si>
   <si>
     <t>double2str</t>
+  </si>
+  <si>
+    <t>./foo/bar/test</t>
+  </si>
+  <si>
+    <t>relative property path 1</t>
+  </si>
+  <si>
+    <t>relative property path 2</t>
   </si>
 </sst>
 </file>
@@ -455,28 +469,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10CA0BE4-5450-449C-8A19-0FD38AB72831}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.53125" customWidth="1"/>
-    <col min="2" max="2" width="13.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.73046875" customWidth="1"/>
-    <col min="5" max="5" width="11.06640625" customWidth="1"/>
-    <col min="6" max="6" width="24.9296875" customWidth="1"/>
-    <col min="7" max="7" width="10.73046875" customWidth="1"/>
-    <col min="8" max="8" width="21.46484375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.53125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.19921875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="25" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -514,10 +529,13 @@
         <v>13</v>
       </c>
       <c r="M1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>123</v>
       </c>
@@ -557,10 +575,13 @@
         <v>3</v>
       </c>
       <c r="M2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>IF(ISBLANK(A2),"",A2)</f>
         <v>123</v>
@@ -605,6 +626,9 @@
         <v>3</v>
       </c>
       <c r="M3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
#2817 /  #2818 - Data Importer fixes and enhancements (#2819)
</commit_message>
<xml_diff>
--- a/bundle/src/test/resources/com/adobe/acs/commons/mcp/impl/processes/data-importer.xlsx
+++ b/bundle/src/test/resources/com/adobe/acs/commons/mcp/impl/processes/data-importer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brobert\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidg/Code/acs-aem-commons/bundle/src/test/resources/com/adobe/acs/commons/mcp/impl/processes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16A6E1C-5A54-43B8-A28D-55C543D5BE8F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A12804D3-2E20-C14B-9E2F-74908ED9CDD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" xr2:uid="{B989199F-66C5-4B28-BA4B-596AA9AB6E6A}"/>
+    <workbookView xWindow="22620" yWindow="14120" windowWidth="34140" windowHeight="12140" xr2:uid="{B989199F-66C5-4B28-BA4B-596AA9AB6E6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>This is just a regular string</t>
   </si>
@@ -81,6 +86,15 @@
   </si>
   <si>
     <t>double2str</t>
+  </si>
+  <si>
+    <t>./foo/bar/test</t>
+  </si>
+  <si>
+    <t>relative property path 1</t>
+  </si>
+  <si>
+    <t>relative property path 2</t>
   </si>
 </sst>
 </file>
@@ -455,28 +469,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10CA0BE4-5450-449C-8A19-0FD38AB72831}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.53125" customWidth="1"/>
-    <col min="2" max="2" width="13.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.73046875" customWidth="1"/>
-    <col min="5" max="5" width="11.06640625" customWidth="1"/>
-    <col min="6" max="6" width="24.9296875" customWidth="1"/>
-    <col min="7" max="7" width="10.73046875" customWidth="1"/>
-    <col min="8" max="8" width="21.46484375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.53125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.19921875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="25" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -514,10 +529,13 @@
         <v>13</v>
       </c>
       <c r="M1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>123</v>
       </c>
@@ -557,10 +575,13 @@
         <v>3</v>
       </c>
       <c r="M2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>IF(ISBLANK(A2),"",A2)</f>
         <v>123</v>
@@ -605,6 +626,9 @@
         <v>3</v>
       </c>
       <c r="M3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Merging ACS Commons master to Derthenier master
</commit_message>
<xml_diff>
--- a/bundle/src/test/resources/com/adobe/acs/commons/mcp/impl/processes/data-importer.xlsx
+++ b/bundle/src/test/resources/com/adobe/acs/commons/mcp/impl/processes/data-importer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brobert\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidg/Code/acs-aem-commons/bundle/src/test/resources/com/adobe/acs/commons/mcp/impl/processes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16A6E1C-5A54-43B8-A28D-55C543D5BE8F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A12804D3-2E20-C14B-9E2F-74908ED9CDD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" xr2:uid="{B989199F-66C5-4B28-BA4B-596AA9AB6E6A}"/>
+    <workbookView xWindow="22620" yWindow="14120" windowWidth="34140" windowHeight="12140" xr2:uid="{B989199F-66C5-4B28-BA4B-596AA9AB6E6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>This is just a regular string</t>
   </si>
@@ -81,6 +86,15 @@
   </si>
   <si>
     <t>double2str</t>
+  </si>
+  <si>
+    <t>./foo/bar/test</t>
+  </si>
+  <si>
+    <t>relative property path 1</t>
+  </si>
+  <si>
+    <t>relative property path 2</t>
   </si>
 </sst>
 </file>
@@ -455,28 +469,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10CA0BE4-5450-449C-8A19-0FD38AB72831}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.53125" customWidth="1"/>
-    <col min="2" max="2" width="13.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.73046875" customWidth="1"/>
-    <col min="5" max="5" width="11.06640625" customWidth="1"/>
-    <col min="6" max="6" width="24.9296875" customWidth="1"/>
-    <col min="7" max="7" width="10.73046875" customWidth="1"/>
-    <col min="8" max="8" width="21.46484375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.53125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.19921875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="25" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -514,10 +529,13 @@
         <v>13</v>
       </c>
       <c r="M1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>123</v>
       </c>
@@ -557,10 +575,13 @@
         <v>3</v>
       </c>
       <c r="M2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>IF(ISBLANK(A2),"",A2)</f>
         <v>123</v>
@@ -605,6 +626,9 @@
         <v>3</v>
       </c>
       <c r="M3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>